<commit_message>
add corresponding author info
</commit_message>
<xml_diff>
--- a/JorunalFinder.xlsx
+++ b/JorunalFinder.xlsx
@@ -1,44 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25619"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Documents\projects\ANT-APCT-Paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A7E4853-E696-453F-ADEA-95932CBE060A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3AD470-9E39-4283-A41B-10617E207DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="307" activeTab="3" xr2:uid="{6FCF1A85-07F8-4469-BD61-1ACE709580B5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="233" activeTab="2" xr2:uid="{6FCF1A85-07F8-4469-BD61-1ACE709580B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Start" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
-    <sheet name="Sorted (Slim)" sheetId="4" r:id="rId3"/>
-    <sheet name="Sorted" sheetId="3" r:id="rId4"/>
+    <sheet name="Sorted" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_num" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">Data!$A$1</definedName>
-    <definedName name="solver_opt" localSheetId="3" hidden="1">Sorted!$A$1</definedName>
-    <definedName name="solver_opt" localSheetId="2" hidden="1">'Sorted (Slim)'!$A$1</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">Sorted!$A$1</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
-    <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -83,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="86">
   <si>
     <t>Where to post my paper?</t>
   </si>
@@ -395,16 +387,10 @@
     <t>Formula definition:</t>
   </si>
   <si>
-    <t>Rev-Time (w)</t>
-  </si>
-  <si>
-    <t>ImpactF</t>
-  </si>
-  <si>
-    <t>3 Journal evaluation sorted… (slim view)</t>
-  </si>
-  <si>
-    <t>SWITCH(C2,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D2/3)+(4/E2)+(2-G2)/1.5+(H2/4)+SWITCH(J2,"No",0,"Yes",0.4)+SWITCH(K2,"No",0,"Low",-1,"Middle",-2)+(L2/3)+SWITCH(M2,"Yes",0.4,"No",0)+(N2*4)+SWITCH(R2,"Recommended",0.4,0)+SWITCH(O2,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E2&gt;=12,-2,0)</t>
+    <t>SWITCH(C2,"Elsevier",1.5,"Springer",0.5,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D2/3)+(4/E2)+(2-G2)+(H2/4)+SWITCH(J2,"No",0,"Yes",0.4)+SWITCH(K2,"No",0,"Low",-1,"Middle",-2)+(L2/3)+SWITCH(M2,"Yes",0.4,"No",0)+(N2*4)+SWITCH(R2,"Recommended",0.4,0)+IF(E2&gt;=12,-2,0)</t>
+  </si>
+  <si>
+    <t>ANNALS OF PURE AND APPLIED LOGIC (SELECTED 🐈)</t>
   </si>
 </sst>
 </file>
@@ -489,7 +475,7 @@
       <name val="Fira Code"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -517,6 +503,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -664,7 +656,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -732,164 +724,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="54">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0066FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="36">
     <dxf>
       <fill>
         <patternFill>
@@ -1217,10 +1058,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1541,7 +1378,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6:L6"/>
+      <selection activeCell="H9" sqref="H9:M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1618,15 +1455,6 @@
       <c r="K6" s="24"/>
       <c r="L6" s="24"/>
     </row>
-    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="H7" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-    </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>82</v>
@@ -1653,7 +1481,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="H9" s="8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
@@ -1732,8 +1560,7 @@
       <c r="M14" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="H7:L7"/>
+  <mergeCells count="9">
     <mergeCell ref="A8:F14"/>
     <mergeCell ref="H9:M14"/>
     <mergeCell ref="H8:M8"/>
@@ -1747,7 +1574,6 @@
   <hyperlinks>
     <hyperlink ref="H5:L5" location="Data!A1" display="1 Journal details collected…" xr:uid="{7C1BCC09-6391-4909-8A22-836AFCC3ABDE}"/>
     <hyperlink ref="H6:L6" location="Sorted!A1" display="2 Journal evaluation sorted…" xr:uid="{F5F3D78C-EA7B-4EB4-A5D6-B27090AA0764}"/>
-    <hyperlink ref="H7:L7" location="'Sorted (Slim)'!A1" display="3 Journal evaluation sorted… (slim view)" xr:uid="{90EC46B7-0F84-4B15-A4ED-25D8557E42FB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2675,34 +2501,34 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A16 I2:I16 M1 C2:G16 C1:K1 P2:R16 O1:R1">
-    <cfRule type="containsText" dxfId="53" priority="23" operator="containsText" text="Recommended">
+    <cfRule type="containsText" dxfId="35" priority="23" operator="containsText" text="Recommended">
       <formula>NOT(ISERROR(SEARCH("Recommended",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="24" operator="containsText" text="Letpub">
+    <cfRule type="containsText" dxfId="34" priority="24" operator="containsText" text="Letpub">
       <formula>NOT(ISERROR(SEARCH("Letpub",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="25" operator="containsText" text="cell">
+    <cfRule type="containsText" dxfId="33" priority="25" operator="containsText" text="cell">
       <formula>NOT(ISERROR(SEARCH("cell",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="26" operator="containsText" text="IEEE">
+    <cfRule type="containsText" dxfId="32" priority="26" operator="containsText" text="IEEE">
       <formula>NOT(ISERROR(SEARCH("IEEE",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="27" operator="containsText" text="sciencedirect">
+    <cfRule type="containsText" dxfId="31" priority="27" operator="containsText" text="sciencedirect">
       <formula>NOT(ISERROR(SEARCH("sciencedirect",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="28" operator="containsText" text="AMS">
+    <cfRule type="containsText" dxfId="30" priority="28" operator="containsText" text="AMS">
       <formula>NOT(ISERROR(SEARCH("AMS",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="29" operator="containsText" text="Wiley">
+    <cfRule type="containsText" dxfId="29" priority="29" operator="containsText" text="Wiley">
       <formula>NOT(ISERROR(SEARCH("Wiley",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="30" operator="containsText" text="MDPI">
+    <cfRule type="containsText" dxfId="28" priority="30" operator="containsText" text="MDPI">
       <formula>NOT(ISERROR(SEARCH("MDPI",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="31" operator="containsText" text="Springer">
+    <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="Springer">
       <formula>NOT(ISERROR(SEARCH("Springer",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="32" operator="containsText" text="Elsevier">
+    <cfRule type="containsText" dxfId="26" priority="32" operator="containsText" text="Elsevier">
       <formula>NOT(ISERROR(SEARCH("Elsevier",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2781,7 +2607,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J16 O2:O16 L2:M16">
-    <cfRule type="containsText" dxfId="43" priority="13" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="25" priority="13" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",J2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2805,22 +2631,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J16 M2:M16">
-    <cfRule type="containsText" dxfId="42" priority="10" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="24" priority="10" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",J2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K16">
-    <cfRule type="containsText" dxfId="41" priority="9" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="23" priority="9" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="containsText" dxfId="40" priority="8" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="22" priority="8" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",K7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14">
-    <cfRule type="containsText" dxfId="39" priority="7" operator="containsText" text="Middle">
+    <cfRule type="containsText" dxfId="21" priority="7" operator="containsText" text="Middle">
       <formula>NOT(ISERROR(SEARCH("Middle",K14)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2839,10 +2665,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O16">
-    <cfRule type="containsText" dxfId="38" priority="4" operator="containsText" text="hard">
+    <cfRule type="containsText" dxfId="20" priority="4" operator="containsText" text="hard">
       <formula>NOT(ISERROR(SEARCH("hard",O2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="5" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="19" priority="5" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2922,1260 +2748,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A16A19E-582D-4D11-92AD-EE569145566A}">
-  <dimension ref="A1:S16"/>
-  <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="160" zoomScalePageLayoutView="10" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="3.88671875" customWidth="1"/>
-    <col min="2" max="2" width="51.44140625" customWidth="1"/>
-    <col min="4" max="4" width="7.44140625" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" customWidth="1"/>
-    <col min="7" max="7" width="2.44140625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" customWidth="1"/>
-    <col min="14" max="14" width="14.77734375" customWidth="1"/>
-    <col min="15" max="15" width="10.5546875" customWidth="1"/>
-    <col min="16" max="16" width="0" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="62.33203125" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="13.21875" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.77600000000000002</v>
-      </c>
-      <c r="E2" s="2">
-        <v>4</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="2">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="3">
-        <v>2</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="S2" s="6" cm="1">
-        <f t="array" ref="S2">_xlfn.SWITCH(C2,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D2/3)+(4/E2)+(2-G2)/1.5+(H2/4)+_xlfn.SWITCH(J2,"No",0,"Yes",0.4)+_xlfn.SWITCH(K2,"No",0,"Low",-1,"Middle",-2)+(L2/3)+_xlfn.SWITCH(M2,"Yes",0.4,"No",0)+(N2*4)+_xlfn.SWITCH(R2,"Recommended",0.4,0)+_xlfn.SWITCH(O2,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E2&gt;=12,-2,0)</f>
-        <v>7.6669999999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="3">
-        <v>2.5920000000000001</v>
-      </c>
-      <c r="E3" s="2">
-        <v>3</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0</v>
-      </c>
-      <c r="H3" s="3">
-        <v>2.9</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="L3" s="3">
-        <v>1</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="N3" s="3">
-        <v>0.69199999999999995</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="S3" s="6" cm="1">
-        <f t="array" ref="S3">_xlfn.SWITCH(C3,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D3/3)+(4/E3)+(2-G3)/1.5+(H3/4)+_xlfn.SWITCH(J3,"No",0,"Yes",0.4)+_xlfn.SWITCH(K3,"No",0,"Low",-1,"Middle",-2)+(L3/3)+_xlfn.SWITCH(M3,"Yes",0.4,"No",0)+(N3*4)+_xlfn.SWITCH(R3,"Recommended",0.4,0)+_xlfn.SWITCH(O3,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E3&gt;=12,-2,0)</f>
-        <v>7.657</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="3">
-        <v>2.8679999999999999</v>
-      </c>
-      <c r="E4" s="2">
-        <v>9</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="2">
-        <v>2</v>
-      </c>
-      <c r="H4" s="3">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" s="3">
-        <v>2</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="N4" s="3">
-        <v>0.61</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="S4" s="6" cm="1">
-        <f t="array" ref="S4">_xlfn.SWITCH(C4,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D4/3)+(4/E4)+(2-G4)/1.5+(H4/4)+_xlfn.SWITCH(J4,"No",0,"Yes",0.4)+_xlfn.SWITCH(K4,"No",0,"Low",-1,"Middle",-2)+(L4/3)+_xlfn.SWITCH(M4,"Yes",0.4,"No",0)+(N4*4)+_xlfn.SWITCH(R4,"Recommended",0.4,0)+_xlfn.SWITCH(O4,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E4&gt;=12,-2,0)</f>
-        <v>7.4321111111111104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="3">
-        <v>3.7759999999999998</v>
-      </c>
-      <c r="E5" s="2">
-        <v>18</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
-      <c r="H5" s="3">
-        <v>4</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L5" s="3">
-        <v>2</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="N5" s="3">
-        <v>0.69199999999999995</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="S5" s="6" cm="1">
-        <f t="array" ref="S5">_xlfn.SWITCH(C5,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D5/3)+(4/E5)+(2-G5)/1.5+(H5/4)+_xlfn.SWITCH(J5,"No",0,"Yes",0.4)+_xlfn.SWITCH(K5,"No",0,"Low",-1,"Middle",-2)+(L5/3)+_xlfn.SWITCH(M5,"Yes",0.4,"No",0)+(N5*4)+_xlfn.SWITCH(R5,"Recommended",0.4,0)+_xlfn.SWITCH(O5,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E5&gt;=12,-2,0)</f>
-        <v>7.1488888888888891</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>13</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="3">
-        <v>4.476</v>
-      </c>
-      <c r="E6" s="2">
-        <v>6</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G6" s="2">
-        <v>2</v>
-      </c>
-      <c r="H6" s="3">
-        <v>6.7</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="L6" s="3">
-        <v>2</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="N6" s="3">
-        <v>0.84</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S6" s="6" cm="1">
-        <f t="array" ref="S6">_xlfn.SWITCH(C6,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D6/3)+(4/E6)+(2-G6)/1.5+(H6/4)+_xlfn.SWITCH(J6,"No",0,"Yes",0.4)+_xlfn.SWITCH(K6,"No",0,"Low",-1,"Middle",-2)+(L6/3)+_xlfn.SWITCH(M6,"Yes",0.4,"No",0)+(N6*4)+_xlfn.SWITCH(R6,"Recommended",0.4,0)+_xlfn.SWITCH(O6,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E6&gt;=12,-2,0)</f>
-        <v>6.7603333333333335</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>8</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="3">
-        <v>4.4619999999999997</v>
-      </c>
-      <c r="E7" s="2">
-        <v>12</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0</v>
-      </c>
-      <c r="H7" s="3">
-        <v>7.1</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L7" s="3">
-        <v>1</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N7" s="3">
-        <v>0.22</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="S7" s="6" cm="1">
-        <f t="array" ref="S7">_xlfn.SWITCH(C7,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D7/3)+(4/E7)+(2-G7)/1.5+(H7/4)+_xlfn.SWITCH(J7,"No",0,"Yes",0.4)+_xlfn.SWITCH(K7,"No",0,"Low",-1,"Middle",-2)+(L7/3)+_xlfn.SWITCH(M7,"Yes",0.4,"No",0)+(N7*4)+_xlfn.SWITCH(R7,"Recommended",0.4,0)+_xlfn.SWITCH(O7,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E7&gt;=12,-2,0)</f>
-        <v>5.9423333333333339</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>14</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1.24</v>
-      </c>
-      <c r="E8" s="2">
-        <v>24</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8" s="3">
-        <v>3</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="N8" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="S8" s="6" cm="1">
-        <f t="array" ref="S8">_xlfn.SWITCH(C8,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D8/3)+(4/E8)+(2-G8)/1.5+(H8/4)+_xlfn.SWITCH(J8,"No",0,"Yes",0.4)+_xlfn.SWITCH(K8,"No",0,"Low",-1,"Middle",-2)+(L8/3)+_xlfn.SWITCH(M8,"Yes",0.4,"No",0)+(N8*4)+_xlfn.SWITCH(R8,"Recommended",0.4,0)+_xlfn.SWITCH(O8,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E8&gt;=12,-2,0)</f>
-        <v>5.7633333333333336</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>12</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1.002</v>
-      </c>
-      <c r="E9" s="2">
-        <v>15</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0</v>
-      </c>
-      <c r="H9" s="3">
-        <v>2.1</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L9" s="3">
-        <v>4</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="N9" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="R9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="S9" s="6" cm="1">
-        <f t="array" ref="S9">_xlfn.SWITCH(C9,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D9/3)+(4/E9)+(2-G9)/1.5+(H9/4)+_xlfn.SWITCH(J9,"No",0,"Yes",0.4)+_xlfn.SWITCH(K9,"No",0,"Low",-1,"Middle",-2)+(L9/3)+_xlfn.SWITCH(M9,"Yes",0.4,"No",0)+(N9*4)+_xlfn.SWITCH(R9,"Recommended",0.4,0)+_xlfn.SWITCH(O9,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E9&gt;=12,-2,0)</f>
-        <v>5.6923333333333339</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="3">
-        <v>5.8360000000000003</v>
-      </c>
-      <c r="E10" s="2">
-        <v>15</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G10" s="2">
-        <v>1</v>
-      </c>
-      <c r="H10" s="3">
-        <v>7.2</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L10" s="3">
-        <v>1</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="N10" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="P10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="R10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="S10" s="6" cm="1">
-        <f t="array" ref="S10">_xlfn.SWITCH(C10,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D10/3)+(4/E10)+(2-G10)/1.5+(H10/4)+_xlfn.SWITCH(J10,"No",0,"Yes",0.4)+_xlfn.SWITCH(K10,"No",0,"Low",-1,"Middle",-2)+(L10/3)+_xlfn.SWITCH(M10,"Yes",0.4,"No",0)+(N10*4)+_xlfn.SWITCH(R10,"Recommended",0.4,0)+_xlfn.SWITCH(O10,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E10&gt;=12,-2,0)</f>
-        <v>5.4119999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>15</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="E11" s="2">
-        <v>12</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0</v>
-      </c>
-      <c r="H11" s="3">
-        <v>4.2</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L11" s="3">
-        <v>4</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="N11" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="R11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S11" s="6" cm="1">
-        <f t="array" ref="S11">_xlfn.SWITCH(C11,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D11/3)+(4/E11)+(2-G11)/1.5+(H11/4)+_xlfn.SWITCH(J11,"No",0,"Yes",0.4)+_xlfn.SWITCH(K11,"No",0,"Low",-1,"Middle",-2)+(L11/3)+_xlfn.SWITCH(M11,"Yes",0.4,"No",0)+(N11*4)+_xlfn.SWITCH(R11,"Recommended",0.4,0)+_xlfn.SWITCH(O11,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E11&gt;=12,-2,0)</f>
-        <v>5.3333333333333321</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>3</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="3">
-        <v>2.8079999999999998</v>
-      </c>
-      <c r="E12" s="2">
-        <v>12</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0</v>
-      </c>
-      <c r="H12" s="3">
-        <v>4</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L12" s="3">
-        <v>1</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N12" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S12" s="6" cm="1">
-        <f t="array" ref="S12">_xlfn.SWITCH(C12,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D12/3)+(4/E12)+(2-G12)/1.5+(H12/4)+_xlfn.SWITCH(J12,"No",0,"Yes",0.4)+_xlfn.SWITCH(K12,"No",0,"Low",-1,"Middle",-2)+(L12/3)+_xlfn.SWITCH(M12,"Yes",0.4,"No",0)+(N12*4)+_xlfn.SWITCH(R12,"Recommended",0.4,0)+_xlfn.SWITCH(O12,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E12&gt;=12,-2,0)</f>
-        <v>5.2360000000000007</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>4</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="3">
-        <v>2.774</v>
-      </c>
-      <c r="E13" s="2">
-        <v>12</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="2">
-        <v>0</v>
-      </c>
-      <c r="H13" s="3">
-        <v>5.8</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L13" s="3">
-        <v>1</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N13" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="P13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S13" s="6" cm="1">
-        <f t="array" ref="S13">_xlfn.SWITCH(C13,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D13/3)+(4/E13)+(2-G13)/1.5+(H13/4)+_xlfn.SWITCH(J13,"No",0,"Yes",0.4)+_xlfn.SWITCH(K13,"No",0,"Low",-1,"Middle",-2)+(L13/3)+_xlfn.SWITCH(M13,"Yes",0.4,"No",0)+(N13*4)+_xlfn.SWITCH(R13,"Recommended",0.4,0)+_xlfn.SWITCH(O13,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E13&gt;=12,-2,0)</f>
-        <v>5.174666666666667</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>11</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0.85099999999999998</v>
-      </c>
-      <c r="E14" s="2">
-        <v>28</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G14" s="2">
-        <v>1</v>
-      </c>
-      <c r="H14" s="3">
-        <v>2.6</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L14" s="3">
-        <v>4</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="N14" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="O14" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="P14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q14" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="R14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="S14" s="6" cm="1">
-        <f t="array" ref="S14">_xlfn.SWITCH(C14,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D14/3)+(4/E14)+(2-G14)/1.5+(H14/4)+_xlfn.SWITCH(J14,"No",0,"Yes",0.4)+_xlfn.SWITCH(K14,"No",0,"Low",-1,"Middle",-2)+(L14/3)+_xlfn.SWITCH(M14,"Yes",0.4,"No",0)+(N14*4)+_xlfn.SWITCH(R14,"Recommended",0.4,0)+_xlfn.SWITCH(O14,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E14&gt;=12,-2,0)</f>
-        <v>4.7765238095238098</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>2</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="3">
-        <v>2.9169999999999998</v>
-      </c>
-      <c r="E15" s="2">
-        <v>12</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="2">
-        <v>0</v>
-      </c>
-      <c r="H15" s="3">
-        <v>8.5</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L15" s="3">
-        <v>1</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N15" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="O15" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="P15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="R15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S15" s="6" cm="1">
-        <f t="array" ref="S15">_xlfn.SWITCH(C15,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D15/3)+(4/E15)+(2-G15)/1.5+(H15/4)+_xlfn.SWITCH(J15,"No",0,"Yes",0.4)+_xlfn.SWITCH(K15,"No",0,"Low",-1,"Middle",-2)+(L15/3)+_xlfn.SWITCH(M15,"Yes",0.4,"No",0)+(N15*4)+_xlfn.SWITCH(R15,"Recommended",0.4,0)+_xlfn.SWITCH(O15,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E15&gt;=12,-2,0)</f>
-        <v>3.9373333333333331</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>10</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0.96099999999999997</v>
-      </c>
-      <c r="E16" s="2">
-        <v>24</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G16" s="2">
-        <v>2</v>
-      </c>
-      <c r="H16" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L16" s="3">
-        <v>3</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="N16" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="O16" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="P16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="R16" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="S16" s="6" cm="1">
-        <f t="array" ref="S16">_xlfn.SWITCH(C16,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D16/3)+(4/E16)+(2-G16)/1.5+(H16/4)+_xlfn.SWITCH(J16,"No",0,"Yes",0.4)+_xlfn.SWITCH(K16,"No",0,"Low",-1,"Middle",-2)+(L16/3)+_xlfn.SWITCH(M16,"Yes",0.4,"No",0)+(N16*4)+_xlfn.SWITCH(R16,"Recommended",0.4,0)+_xlfn.SWITCH(O16,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E16&gt;=12,-2,0)</f>
-        <v>3.5620000000000003</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A1:A16 I2:I16 M1 C2:G16 C1:K1 P2:R16 O1:S1">
-    <cfRule type="containsText" dxfId="35" priority="20" operator="containsText" text="Recommended">
-      <formula>NOT(ISERROR(SEARCH("Recommended",A1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="21" operator="containsText" text="Letpub">
-      <formula>NOT(ISERROR(SEARCH("Letpub",A1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="22" operator="containsText" text="cell">
-      <formula>NOT(ISERROR(SEARCH("cell",A1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="23" operator="containsText" text="IEEE">
-      <formula>NOT(ISERROR(SEARCH("IEEE",A1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="24" operator="containsText" text="sciencedirect">
-      <formula>NOT(ISERROR(SEARCH("sciencedirect",A1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="25" operator="containsText" text="AMS">
-      <formula>NOT(ISERROR(SEARCH("AMS",A1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="26" operator="containsText" text="Wiley">
-      <formula>NOT(ISERROR(SEARCH("Wiley",A1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="27" operator="containsText" text="MDPI">
-      <formula>NOT(ISERROR(SEARCH("MDPI",A1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="28" operator="containsText" text="Springer">
-      <formula>NOT(ISERROR(SEARCH("Springer",A1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="29" operator="containsText" text="Elsevier">
-      <formula>NOT(ISERROR(SEARCH("Elsevier",A1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D16">
-    <cfRule type="dataBar" priority="19">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF1FD3BE"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{168F2759-4A3B-4944-90D0-79B9A965C26F}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E16">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF77F874"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFEE6E6E"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF00B050"/>
-        <color rgb="FFFFFF00"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:G16">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF77F874"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFEE6E6E"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I16 P2:P16">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF77F874"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFEE6E6E"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H16">
-    <cfRule type="dataBar" priority="14">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF1FD3BE"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3EDAABBA-E6C3-4DA9-B9A2-89E898983B4A}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L16">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF77F874"/>
-        <color rgb="FFCFFAC2"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="iconSet" priority="13">
-      <iconSet iconSet="5Rating" reverse="1">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="2"/>
-        <cfvo type="num" val="3"/>
-        <cfvo type="num" val="4"/>
-        <cfvo type="num" val="5"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J16 M2:M16">
-    <cfRule type="containsText" dxfId="25" priority="1" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",J2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="11" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH("No",J2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K16">
-    <cfRule type="containsText" dxfId="23" priority="8" operator="containsText" text="Middle">
-      <formula>NOT(ISERROR(SEARCH("Middle",K2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="9" operator="containsText" text="Low">
-      <formula>NOT(ISERROR(SEARCH("Low",K2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="10" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH("No",K2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N16">
-    <cfRule type="dataBar" priority="7">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF1FD3BE"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{92FD3632-A1CD-41B0-AD9F-0C2803504CB1}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O2:O16">
-    <cfRule type="containsText" dxfId="20" priority="2" operator="containsText" text="Middle">
-      <formula>NOT(ISERROR(SEARCH("Middle",O2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="5" operator="containsText" text="hard">
-      <formula>NOT(ISERROR(SEARCH("hard",O2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="6" operator="containsText" text="Easy">
-      <formula>NOT(ISERROR(SEARCH("Easy",O2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S16">
-    <cfRule type="iconSet" priority="3">
-      <iconSet iconSet="5Rating">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="20"/>
-        <cfvo type="percent" val="40"/>
-        <cfvo type="percent" val="60"/>
-        <cfvo type="percent" val="80"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="dataBar" priority="4">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF1FD3BE"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{21B80AC1-A68F-43F9-AB31-FD11D787722F}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1" xr:uid="{C41D68B1-D034-4EC5-B436-4A7D328AAF09}"/>
-    <hyperlink ref="P15" r:id="rId2" xr:uid="{57836E9A-4F95-4D8F-A45F-0EAAAF2AF1CF}"/>
-    <hyperlink ref="P12" r:id="rId3" xr:uid="{AC931194-55CC-4053-B70B-AD05E65CC567}"/>
-    <hyperlink ref="P13" r:id="rId4" xr:uid="{BAB0CF3C-8B4C-417A-BAFD-3183047D05D9}"/>
-    <hyperlink ref="P4" r:id="rId5" xr:uid="{3E7C6D6B-08E4-4CAB-90A9-3253DBDE0553}"/>
-    <hyperlink ref="P3" r:id="rId6" xr:uid="{41F09A90-CF30-47E2-A3DC-5B56C27A339F}"/>
-    <hyperlink ref="P5" r:id="rId7" xr:uid="{697A2BAE-D171-4D08-958E-C630EE534B4C}"/>
-    <hyperlink ref="P7" r:id="rId8" xr:uid="{F6C603EA-3791-445A-B30E-49A3D0DA08A1}"/>
-    <hyperlink ref="P10" r:id="rId9" xr:uid="{702B2E3E-ADB5-46F8-9544-93CF581465F4}"/>
-    <hyperlink ref="P16" r:id="rId10" xr:uid="{A3890CC8-F652-4558-864B-33D9FB4FD2C2}"/>
-    <hyperlink ref="P14" r:id="rId11" xr:uid="{490550A6-081F-4EC8-AA89-8B0DD2125558}"/>
-    <hyperlink ref="P9" r:id="rId12" xr:uid="{6C5D2D3C-F229-4559-8D24-A85508DF9F02}"/>
-    <hyperlink ref="P6" r:id="rId13" xr:uid="{82EBABD4-F092-4AA7-B9AF-3A53C2DE855C}"/>
-    <hyperlink ref="P8" r:id="rId14" xr:uid="{A22B345E-7C9B-4763-BF1C-107C0C903C21}"/>
-    <hyperlink ref="P11" r:id="rId15" xr:uid="{7FD26781-076F-4BD4-B9AB-A5BAB8397886}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{168F2759-4A3B-4944-90D0-79B9A965C26F}">
-            <x14:dataBar minLength="0" maxLength="100">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D2:D16</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3EDAABBA-E6C3-4DA9-B9A2-89E898983B4A}">
-            <x14:dataBar minLength="0" maxLength="100">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>H2:H16</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{92FD3632-A1CD-41B0-AD9F-0C2803504CB1}">
-            <x14:dataBar minLength="0" maxLength="100">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>N2:N16</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{21B80AC1-A68F-43F9-AB31-FD11D787722F}">
-            <x14:dataBar minLength="0" maxLength="100">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>S2:S16</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55C9DC25-BC57-41A3-9745-57893597D3F6}">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="160" zoomScalePageLayoutView="10" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="130" zoomScaleSheetLayoutView="160" zoomScalePageLayoutView="10" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4253,11 +2830,11 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="A2" s="27">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
+      <c r="B2" s="27" t="s">
+        <v>85</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -4308,8 +2885,8 @@
         <v>24</v>
       </c>
       <c r="S2" s="6" cm="1">
-        <f t="array" ref="S2">_xlfn.SWITCH(C2,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D2/3)+(4/E2)+(2-G2)/1.5+(H2/4)+_xlfn.SWITCH(J2,"No",0,"Yes",0.4)+_xlfn.SWITCH(K2,"No",0,"Low",-1,"Middle",-2)+(L2/3)+_xlfn.SWITCH(M2,"Yes",0.4,"No",0)+(N2*4)+_xlfn.SWITCH(R2,"Recommended",0.4,0)+_xlfn.SWITCH(O2,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E2&gt;=12,-2,0)</f>
-        <v>7.6669999999999998</v>
+        <f t="array" ref="S2">_xlfn.SWITCH(C2,"Elsevier",1.5,"Springer",0.5,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D2/3)+(4/E2)+(2-G2)+(H2/4)+_xlfn.SWITCH(J2,"No",0,"Yes",0.4)+_xlfn.SWITCH(K2,"No",0,"Low",-1,"Middle",-2)+(L2/3)+_xlfn.SWITCH(M2,"Yes",0.4,"No",0)+(N2*4)+_xlfn.SWITCH(R2,"Recommended",0.4,0)+IF(E2&gt;=12,-2,0)</f>
+        <v>8.0003333333333337</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
@@ -4368,34 +2945,34 @@
         <v>24</v>
       </c>
       <c r="S3" s="6" cm="1">
-        <f t="array" ref="S3">_xlfn.SWITCH(C3,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D3/3)+(4/E3)+(2-G3)/1.5+(H3/4)+_xlfn.SWITCH(J3,"No",0,"Yes",0.4)+_xlfn.SWITCH(K3,"No",0,"Low",-1,"Middle",-2)+(L3/3)+_xlfn.SWITCH(M3,"Yes",0.4,"No",0)+(N3*4)+_xlfn.SWITCH(R3,"Recommended",0.4,0)+_xlfn.SWITCH(O3,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E3&gt;=12,-2,0)</f>
-        <v>7.657</v>
+        <f t="array" ref="S3">_xlfn.SWITCH(C3,"Elsevier",1.5,"Springer",0.5,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D3/3)+(4/E3)+(2-G3)/1.2+(H3/4)+_xlfn.SWITCH(J3,"No",0,"Yes",0.4)+_xlfn.SWITCH(K3,"No",0,"Low",-1,"Middle",-2)+(L3/3)+_xlfn.SWITCH(M3,"Yes",0.4,"No",0)+(N3*4)+_xlfn.SWITCH(R3,"Recommended",0.4,0)+IF(E3&gt;=12,-2,0)</f>
+        <v>7.4903333333333331</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="3">
-        <v>2.8679999999999999</v>
+        <v>3.7759999999999998</v>
       </c>
       <c r="E4" s="2">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G4" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H4" s="3">
-        <v>4.0999999999999996</v>
+        <v>4</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>29</v>
@@ -4413,7 +2990,7 @@
         <v>13</v>
       </c>
       <c r="N4" s="3">
-        <v>0.61</v>
+        <v>0.69199999999999995</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>18</v>
@@ -4422,40 +2999,40 @@
         <v>20</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="R4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="S4" s="6" cm="1">
-        <f t="array" ref="S4">_xlfn.SWITCH(C4,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D4/3)+(4/E4)+(2-G4)/1.5+(H4/4)+_xlfn.SWITCH(J4,"No",0,"Yes",0.4)+_xlfn.SWITCH(K4,"No",0,"Low",-1,"Middle",-2)+(L4/3)+_xlfn.SWITCH(M4,"Yes",0.4,"No",0)+(N4*4)+_xlfn.SWITCH(R4,"Recommended",0.4,0)+_xlfn.SWITCH(O4,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E4&gt;=12,-2,0)</f>
-        <v>7.4321111111111104</v>
+        <f t="array" ref="S4">_xlfn.SWITCH(C4,"Elsevier",1.5,"Springer",0.5,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D4/3)+(4/E4)+(2-G4)/1.2+(H4/4)+_xlfn.SWITCH(J4,"No",0,"Yes",0.4)+_xlfn.SWITCH(K4,"No",0,"Low",-1,"Middle",-2)+(L4/3)+_xlfn.SWITCH(M4,"Yes",0.4,"No",0)+(N4*4)+_xlfn.SWITCH(R4,"Recommended",0.4,0)+IF(E4&gt;=12,-2,0)</f>
+        <v>7.482222222222223</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="3">
-        <v>3.7759999999999998</v>
+        <v>2.8679999999999999</v>
       </c>
       <c r="E5" s="2">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G5" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H5" s="3">
-        <v>4</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>29</v>
@@ -4473,7 +3050,7 @@
         <v>13</v>
       </c>
       <c r="N5" s="3">
-        <v>0.69199999999999995</v>
+        <v>0.61</v>
       </c>
       <c r="O5" s="3" t="s">
         <v>18</v>
@@ -4482,40 +3059,40 @@
         <v>20</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="R5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="S5" s="6" cm="1">
-        <f t="array" ref="S5">_xlfn.SWITCH(C5,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D5/3)+(4/E5)+(2-G5)/1.5+(H5/4)+_xlfn.SWITCH(J5,"No",0,"Yes",0.4)+_xlfn.SWITCH(K5,"No",0,"Low",-1,"Middle",-2)+(L5/3)+_xlfn.SWITCH(M5,"Yes",0.4,"No",0)+(N5*4)+_xlfn.SWITCH(R5,"Recommended",0.4,0)+_xlfn.SWITCH(O5,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E5&gt;=12,-2,0)</f>
-        <v>7.1488888888888891</v>
+        <f t="array" ref="S5">_xlfn.SWITCH(C5,"Elsevier",1.5,"Springer",0.5,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D5/3)+(4/E5)+(2-G5)/1.2+(H5/4)+_xlfn.SWITCH(J5,"No",0,"Yes",0.4)+_xlfn.SWITCH(K5,"No",0,"Low",-1,"Middle",-2)+(L5/3)+_xlfn.SWITCH(M5,"Yes",0.4,"No",0)+(N5*4)+_xlfn.SWITCH(R5,"Recommended",0.4,0)+IF(E5&gt;=12,-2,0)</f>
+        <v>7.4321111111111104</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>66</v>
+        <v>5</v>
       </c>
       <c r="D6" s="3">
-        <v>4.476</v>
+        <v>4.4619999999999997</v>
       </c>
       <c r="E6" s="2">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G6" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H6" s="3">
-        <v>6.7</v>
+        <v>7.1</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>29</v>
@@ -4524,58 +3101,58 @@
         <v>16</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="L6" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="N6" s="3">
-        <v>0.84</v>
+        <v>0.22</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="P6" s="4" t="s">
         <v>20</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="S6" s="6" cm="1">
-        <f t="array" ref="S6">_xlfn.SWITCH(C6,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D6/3)+(4/E6)+(2-G6)/1.5+(H6/4)+_xlfn.SWITCH(J6,"No",0,"Yes",0.4)+_xlfn.SWITCH(K6,"No",0,"Low",-1,"Middle",-2)+(L6/3)+_xlfn.SWITCH(M6,"Yes",0.4,"No",0)+(N6*4)+_xlfn.SWITCH(R6,"Recommended",0.4,0)+_xlfn.SWITCH(O6,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E6&gt;=12,-2,0)</f>
-        <v>6.7603333333333335</v>
+        <f t="array" ref="S6">_xlfn.SWITCH(C6,"Elsevier",1.5,"Springer",0.5,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D6/3)+(4/E6)+(2-G6)/1.2+(H6/4)+_xlfn.SWITCH(J6,"No",0,"Yes",0.4)+_xlfn.SWITCH(K6,"No",0,"Low",-1,"Middle",-2)+(L6/3)+_xlfn.SWITCH(M6,"Yes",0.4,"No",0)+(N6*4)+_xlfn.SWITCH(R6,"Recommended",0.4,0)+IF(E6&gt;=12,-2,0)</f>
+        <v>6.7756666666666661</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="D7" s="3">
-        <v>4.4619999999999997</v>
+        <v>4.476</v>
       </c>
       <c r="E7" s="2">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="G7" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H7" s="3">
-        <v>7.1</v>
+        <v>6.7</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>29</v>
@@ -4584,32 +3161,32 @@
         <v>16</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="L7" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="N7" s="3">
-        <v>0.22</v>
+        <v>0.84</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="P7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="S7" s="6" cm="1">
-        <f t="array" ref="S7">_xlfn.SWITCH(C7,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D7/3)+(4/E7)+(2-G7)/1.5+(H7/4)+_xlfn.SWITCH(J7,"No",0,"Yes",0.4)+_xlfn.SWITCH(K7,"No",0,"Low",-1,"Middle",-2)+(L7/3)+_xlfn.SWITCH(M7,"Yes",0.4,"No",0)+(N7*4)+_xlfn.SWITCH(R7,"Recommended",0.4,0)+_xlfn.SWITCH(O7,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E7&gt;=12,-2,0)</f>
-        <v>5.9423333333333339</v>
+        <f t="array" ref="S7">_xlfn.SWITCH(C7,"Elsevier",1.5,"Springer",0.5,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D7/3)+(4/E7)+(2-G7)/1.2+(H7/4)+_xlfn.SWITCH(J7,"No",0,"Yes",0.4)+_xlfn.SWITCH(K7,"No",0,"Low",-1,"Middle",-2)+(L7/3)+_xlfn.SWITCH(M7,"Yes",0.4,"No",0)+(N7*4)+_xlfn.SWITCH(R7,"Recommended",0.4,0)+IF(E7&gt;=12,-2,0)</f>
+        <v>6.2603333333333335</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
@@ -4668,34 +3245,34 @@
         <v>24</v>
       </c>
       <c r="S8" s="6" cm="1">
-        <f t="array" ref="S8">_xlfn.SWITCH(C8,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D8/3)+(4/E8)+(2-G8)/1.5+(H8/4)+_xlfn.SWITCH(J8,"No",0,"Yes",0.4)+_xlfn.SWITCH(K8,"No",0,"Low",-1,"Middle",-2)+(L8/3)+_xlfn.SWITCH(M8,"Yes",0.4,"No",0)+(N8*4)+_xlfn.SWITCH(R8,"Recommended",0.4,0)+_xlfn.SWITCH(O8,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E8&gt;=12,-2,0)</f>
-        <v>5.7633333333333336</v>
+        <f t="array" ref="S8">_xlfn.SWITCH(C8,"Elsevier",1.5,"Springer",0.5,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D8/3)+(4/E8)+(2-G8)/1.2+(H8/4)+_xlfn.SWITCH(J8,"No",0,"Yes",0.4)+_xlfn.SWITCH(K8,"No",0,"Low",-1,"Middle",-2)+(L8/3)+_xlfn.SWITCH(M8,"Yes",0.4,"No",0)+(N8*4)+_xlfn.SWITCH(R8,"Recommended",0.4,0)+IF(E8&gt;=12,-2,0)</f>
+        <v>6.0966666666666676</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="3">
-        <v>1.002</v>
+        <v>5.8360000000000003</v>
       </c>
       <c r="E9" s="2">
         <v>15</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="3">
-        <v>2.1</v>
+        <v>7.2</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>11</v>
@@ -4707,55 +3284,55 @@
         <v>13</v>
       </c>
       <c r="L9" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="N9" s="3">
-        <v>0.6</v>
+        <v>0.25</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="P9" s="4" t="s">
         <v>20</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="S9" s="6" cm="1">
-        <f t="array" ref="S9">_xlfn.SWITCH(C9,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D9/3)+(4/E9)+(2-G9)/1.5+(H9/4)+_xlfn.SWITCH(J9,"No",0,"Yes",0.4)+_xlfn.SWITCH(K9,"No",0,"Low",-1,"Middle",-2)+(L9/3)+_xlfn.SWITCH(M9,"Yes",0.4,"No",0)+(N9*4)+_xlfn.SWITCH(R9,"Recommended",0.4,0)+_xlfn.SWITCH(O9,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E9&gt;=12,-2,0)</f>
-        <v>5.6923333333333339</v>
+        <f t="array" ref="S9">_xlfn.SWITCH(C9,"Elsevier",1.5,"Springer",0.5,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D9/3)+(4/E9)+(2-G9)/1.2+(H9/4)+_xlfn.SWITCH(J9,"No",0,"Yes",0.4)+_xlfn.SWITCH(K9,"No",0,"Low",-1,"Middle",-2)+(L9/3)+_xlfn.SWITCH(M9,"Yes",0.4,"No",0)+(N9*4)+_xlfn.SWITCH(R9,"Recommended",0.4,0)+IF(E9&gt;=12,-2,0)</f>
+        <v>6.0786666666666651</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="3">
-        <v>5.8360000000000003</v>
+        <v>1.002</v>
       </c>
       <c r="E10" s="2">
         <v>15</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="3">
-        <v>7.2</v>
+        <v>2.1</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>11</v>
@@ -4767,29 +3344,29 @@
         <v>13</v>
       </c>
       <c r="L10" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M10" s="3" t="s">
         <v>13</v>
       </c>
       <c r="N10" s="3">
-        <v>0.25</v>
+        <v>0.6</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="P10" s="4" t="s">
         <v>20</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="S10" s="6" cm="1">
-        <f t="array" ref="S10">_xlfn.SWITCH(C10,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D10/3)+(4/E10)+(2-G10)/1.5+(H10/4)+_xlfn.SWITCH(J10,"No",0,"Yes",0.4)+_xlfn.SWITCH(K10,"No",0,"Low",-1,"Middle",-2)+(L10/3)+_xlfn.SWITCH(M10,"Yes",0.4,"No",0)+(N10*4)+_xlfn.SWITCH(R10,"Recommended",0.4,0)+_xlfn.SWITCH(O10,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E10&gt;=12,-2,0)</f>
-        <v>5.4119999999999999</v>
+        <f t="array" ref="S10">_xlfn.SWITCH(C10,"Elsevier",1.5,"Springer",0.5,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D10/3)+(4/E10)+(2-G10)/1.2+(H10/4)+_xlfn.SWITCH(J10,"No",0,"Yes",0.4)+_xlfn.SWITCH(K10,"No",0,"Low",-1,"Middle",-2)+(L10/3)+_xlfn.SWITCH(M10,"Yes",0.4,"No",0)+(N10*4)+_xlfn.SWITCH(R10,"Recommended",0.4,0)+IF(E10&gt;=12,-2,0)</f>
+        <v>6.0256666666666661</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
@@ -4848,22 +3425,22 @@
         <v>32</v>
       </c>
       <c r="S11" s="6" cm="1">
-        <f t="array" ref="S11">_xlfn.SWITCH(C11,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D11/3)+(4/E11)+(2-G11)/1.5+(H11/4)+_xlfn.SWITCH(J11,"No",0,"Yes",0.4)+_xlfn.SWITCH(K11,"No",0,"Low",-1,"Middle",-2)+(L11/3)+_xlfn.SWITCH(M11,"Yes",0.4,"No",0)+(N11*4)+_xlfn.SWITCH(R11,"Recommended",0.4,0)+_xlfn.SWITCH(O11,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E11&gt;=12,-2,0)</f>
-        <v>5.3333333333333321</v>
+        <f t="array" ref="S11">_xlfn.SWITCH(C11,"Elsevier",1.5,"Springer",0.5,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D11/3)+(4/E11)+(2-G11)/1.2+(H11/4)+_xlfn.SWITCH(J11,"No",0,"Yes",0.4)+_xlfn.SWITCH(K11,"No",0,"Low",-1,"Middle",-2)+(L11/3)+_xlfn.SWITCH(M11,"Yes",0.4,"No",0)+(N11*4)+_xlfn.SWITCH(R11,"Recommended",0.4,0)+IF(E11&gt;=12,-2,0)</f>
+        <v>5.6666666666666661</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D12" s="3">
-        <v>2.8079999999999998</v>
+        <v>2.774</v>
       </c>
       <c r="E12" s="2">
         <v>12</v>
@@ -4875,7 +3452,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="3">
-        <v>4</v>
+        <v>5.8</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>29</v>
@@ -4896,140 +3473,140 @@
         <v>0.6</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="P12" s="4" t="s">
         <v>20</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="R12" s="2" t="s">
         <v>32</v>
       </c>
       <c r="S12" s="6" cm="1">
-        <f t="array" ref="S12">_xlfn.SWITCH(C12,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D12/3)+(4/E12)+(2-G12)/1.5+(H12/4)+_xlfn.SWITCH(J12,"No",0,"Yes",0.4)+_xlfn.SWITCH(K12,"No",0,"Low",-1,"Middle",-2)+(L12/3)+_xlfn.SWITCH(M12,"Yes",0.4,"No",0)+(N12*4)+_xlfn.SWITCH(R12,"Recommended",0.4,0)+_xlfn.SWITCH(O12,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E12&gt;=12,-2,0)</f>
-        <v>5.2360000000000007</v>
+        <f t="array" ref="S12">_xlfn.SWITCH(C12,"Elsevier",1.5,"Springer",0.5,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D12/3)+(4/E12)+(2-G12)/1.2+(H12/4)+_xlfn.SWITCH(J12,"No",0,"Yes",0.4)+_xlfn.SWITCH(K12,"No",0,"Low",-1,"Middle",-2)+(L12/3)+_xlfn.SWITCH(M12,"Yes",0.4,"No",0)+(N12*4)+_xlfn.SWITCH(R12,"Recommended",0.4,0)+IF(E12&gt;=12,-2,0)</f>
+        <v>5.5080000000000009</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="E13" s="2">
+        <v>28</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3">
+        <v>2.6</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13" s="3">
         <v>4</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="3">
-        <v>2.774</v>
-      </c>
-      <c r="E13" s="2">
-        <v>12</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="2">
-        <v>0</v>
-      </c>
-      <c r="H13" s="3">
-        <v>5.8</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L13" s="3">
-        <v>1</v>
-      </c>
       <c r="M13" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="N13" s="3">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="P13" s="4" t="s">
         <v>20</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="S13" s="6" cm="1">
-        <f t="array" ref="S13">_xlfn.SWITCH(C13,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D13/3)+(4/E13)+(2-G13)/1.5+(H13/4)+_xlfn.SWITCH(J13,"No",0,"Yes",0.4)+_xlfn.SWITCH(K13,"No",0,"Low",-1,"Middle",-2)+(L13/3)+_xlfn.SWITCH(M13,"Yes",0.4,"No",0)+(N13*4)+_xlfn.SWITCH(R13,"Recommended",0.4,0)+_xlfn.SWITCH(O13,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E13&gt;=12,-2,0)</f>
-        <v>5.174666666666667</v>
+        <f t="array" ref="S13">_xlfn.SWITCH(C13,"Elsevier",1.5,"Springer",0.5,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D13/3)+(4/E13)+(2-G13)/1.2+(H13/4)+_xlfn.SWITCH(J13,"No",0,"Yes",0.4)+_xlfn.SWITCH(K13,"No",0,"Low",-1,"Middle",-2)+(L13/3)+_xlfn.SWITCH(M13,"Yes",0.4,"No",0)+(N13*4)+_xlfn.SWITCH(R13,"Recommended",0.4,0)+IF(E13&gt;=12,-2,0)</f>
+        <v>5.1431904761904761</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="D14" s="3">
-        <v>0.85099999999999998</v>
+        <v>2.8079999999999998</v>
       </c>
       <c r="E14" s="2">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>4</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14" s="3">
         <v>1</v>
       </c>
-      <c r="H14" s="3">
-        <v>2.6</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L14" s="3">
-        <v>4</v>
-      </c>
       <c r="M14" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="N14" s="3">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="P14" s="4" t="s">
         <v>20</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="S14" s="6" cm="1">
-        <f t="array" ref="S14">_xlfn.SWITCH(C14,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D14/3)+(4/E14)+(2-G14)/1.5+(H14/4)+_xlfn.SWITCH(J14,"No",0,"Yes",0.4)+_xlfn.SWITCH(K14,"No",0,"Low",-1,"Middle",-2)+(L14/3)+_xlfn.SWITCH(M14,"Yes",0.4,"No",0)+(N14*4)+_xlfn.SWITCH(R14,"Recommended",0.4,0)+_xlfn.SWITCH(O14,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E14&gt;=12,-2,0)</f>
-        <v>4.7765238095238098</v>
+        <f t="array" ref="S14">_xlfn.SWITCH(C14,"Elsevier",1.5,"Springer",0.5,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D14/3)+(4/E14)+(2-G14)/1.2+(H14/4)+_xlfn.SWITCH(J14,"No",0,"Yes",0.4)+_xlfn.SWITCH(K14,"No",0,"Low",-1,"Middle",-2)+(L14/3)+_xlfn.SWITCH(M14,"Yes",0.4,"No",0)+(N14*4)+_xlfn.SWITCH(R14,"Recommended",0.4,0)+IF(E14&gt;=12,-2,0)</f>
+        <v>5.0693333333333328</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
@@ -5088,8 +3665,8 @@
         <v>32</v>
       </c>
       <c r="S15" s="6" cm="1">
-        <f t="array" ref="S15">_xlfn.SWITCH(C15,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D15/3)+(4/E15)+(2-G15)/1.5+(H15/4)+_xlfn.SWITCH(J15,"No",0,"Yes",0.4)+_xlfn.SWITCH(K15,"No",0,"Low",-1,"Middle",-2)+(L15/3)+_xlfn.SWITCH(M15,"Yes",0.4,"No",0)+(N15*4)+_xlfn.SWITCH(R15,"Recommended",0.4,0)+_xlfn.SWITCH(O15,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E15&gt;=12,-2,0)</f>
-        <v>3.9373333333333331</v>
+        <f t="array" ref="S15">_xlfn.SWITCH(C15,"Elsevier",1.5,"Springer",0.5,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D15/3)+(4/E15)+(2-G15)/1.2+(H15/4)+_xlfn.SWITCH(J15,"No",0,"Yes",0.4)+_xlfn.SWITCH(K15,"No",0,"Low",-1,"Middle",-2)+(L15/3)+_xlfn.SWITCH(M15,"Yes",0.4,"No",0)+(N15*4)+_xlfn.SWITCH(R15,"Recommended",0.4,0)+IF(E15&gt;=12,-2,0)</f>
+        <v>4.2706666666666671</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
@@ -5148,15 +3725,15 @@
         <v>24</v>
       </c>
       <c r="S16" s="6" cm="1">
-        <f t="array" ref="S16">_xlfn.SWITCH(C16,"Elsevier",1,"Springer",0,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D16/3)+(4/E16)+(2-G16)/1.5+(H16/4)+_xlfn.SWITCH(J16,"No",0,"Yes",0.4)+_xlfn.SWITCH(K16,"No",0,"Low",-1,"Middle",-2)+(L16/3)+_xlfn.SWITCH(M16,"Yes",0.4,"No",0)+(N16*4)+_xlfn.SWITCH(R16,"Recommended",0.4,0)+_xlfn.SWITCH(O16,"Easy",0.5,"Middle",0.3,"Hard",0)+IF(E16&gt;=12,-2,0)</f>
-        <v>3.5620000000000003</v>
+        <f t="array" ref="S16">_xlfn.SWITCH(C16,"Elsevier",1.5,"Springer",0.5,"MDPI",0,"IEEE",0,"AMS",0,"Wiley",0)+(D16/3)+(4/E16)+(2-G16)/1.2+(H16/4)+_xlfn.SWITCH(J16,"No",0,"Yes",0.4)+_xlfn.SWITCH(K16,"No",0,"Low",-1,"Middle",-2)+(L16/3)+_xlfn.SWITCH(M16,"Yes",0.4,"No",0)+(N16*4)+_xlfn.SWITCH(R16,"Recommended",0.4,0)+IF(E16&gt;=12,-2,0)</f>
+        <v>3.7620000000000005</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S16">
     <sortCondition descending="1" ref="S2:S16"/>
   </sortState>
-  <conditionalFormatting sqref="A1:A16 I2:I16 M1 C2:G16 C1:K1 P2:R16 O1:S1">
+  <conditionalFormatting sqref="A1:A16 M1 C2:G16 C1:K1 P2:R16 O1:S1 I2:I16">
     <cfRule type="containsText" dxfId="17" priority="22" operator="containsText" text="Recommended">
       <formula>NOT(ISERROR(SEARCH("Recommended",A1)))</formula>
     </cfRule>
@@ -5236,7 +3813,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I16 P2:P16">
+  <conditionalFormatting sqref="P2:P16 I2:I16">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -5351,17 +3928,17 @@
   <hyperlinks>
     <hyperlink ref="P2" r:id="rId1" xr:uid="{99E080D1-9D2C-41AE-AC61-8D10F2136019}"/>
     <hyperlink ref="P15" r:id="rId2" xr:uid="{C03C912E-FEDB-4D6F-A870-ED2C7C012E4B}"/>
-    <hyperlink ref="P12" r:id="rId3" xr:uid="{F2006380-6C23-4E6B-8100-F20903194ECC}"/>
-    <hyperlink ref="P13" r:id="rId4" xr:uid="{EC5160FC-99A0-4B03-B206-F1B7E4C579C0}"/>
-    <hyperlink ref="P4" r:id="rId5" xr:uid="{F6F0FF5F-F70B-4BBB-BAC0-105E55F8DEC1}"/>
+    <hyperlink ref="P14" r:id="rId3" xr:uid="{F2006380-6C23-4E6B-8100-F20903194ECC}"/>
+    <hyperlink ref="P12" r:id="rId4" xr:uid="{EC5160FC-99A0-4B03-B206-F1B7E4C579C0}"/>
+    <hyperlink ref="P5" r:id="rId5" xr:uid="{F6F0FF5F-F70B-4BBB-BAC0-105E55F8DEC1}"/>
     <hyperlink ref="P3" r:id="rId6" xr:uid="{45DE32FC-6D7A-459A-B182-7430EE2114A5}"/>
-    <hyperlink ref="P5" r:id="rId7" xr:uid="{C22A1877-304F-4BAC-B048-D159E40DCF6F}"/>
-    <hyperlink ref="P7" r:id="rId8" xr:uid="{027918AB-32BC-498D-A4A5-428C1913B03A}"/>
-    <hyperlink ref="P10" r:id="rId9" xr:uid="{184D8DE2-0385-4828-8BF3-7E86032D0169}"/>
+    <hyperlink ref="P4" r:id="rId7" xr:uid="{C22A1877-304F-4BAC-B048-D159E40DCF6F}"/>
+    <hyperlink ref="P6" r:id="rId8" xr:uid="{027918AB-32BC-498D-A4A5-428C1913B03A}"/>
+    <hyperlink ref="P9" r:id="rId9" xr:uid="{184D8DE2-0385-4828-8BF3-7E86032D0169}"/>
     <hyperlink ref="P16" r:id="rId10" xr:uid="{713EFA22-7222-4B8D-A893-A5CB87FF14D4}"/>
-    <hyperlink ref="P14" r:id="rId11" xr:uid="{D706ABCE-F0FA-48EF-8887-BE6ABB83D53A}"/>
-    <hyperlink ref="P9" r:id="rId12" xr:uid="{13CEE478-7EF0-43AA-83A2-B2DCE121D38F}"/>
-    <hyperlink ref="P6" r:id="rId13" xr:uid="{CAA747B1-6901-436B-AFAB-19D92FB86C50}"/>
+    <hyperlink ref="P13" r:id="rId11" xr:uid="{D706ABCE-F0FA-48EF-8887-BE6ABB83D53A}"/>
+    <hyperlink ref="P10" r:id="rId12" xr:uid="{13CEE478-7EF0-43AA-83A2-B2DCE121D38F}"/>
+    <hyperlink ref="P7" r:id="rId13" xr:uid="{CAA747B1-6901-436B-AFAB-19D92FB86C50}"/>
     <hyperlink ref="P8" r:id="rId14" xr:uid="{B9C0B575-16F9-45BB-ABE7-7C869AF0BEED}"/>
     <hyperlink ref="P11" r:id="rId15" xr:uid="{11F8BC0E-4D4A-4639-B9B1-DFBA74031C7F}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
remove notebook file from master
</commit_message>
<xml_diff>
--- a/JorunalFinder.xlsx
+++ b/JorunalFinder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Documents\projects\ANT-APCT-Paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3AD470-9E39-4283-A41B-10617E207DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E369B821-01EE-4CCA-B21D-7B7EBA023DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="233" activeTab="2" xr2:uid="{6FCF1A85-07F8-4469-BD61-1ACE709580B5}"/>
   </bookViews>
@@ -664,6 +664,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -724,7 +725,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1384,180 +1384,180 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="H2" s="25" t="s">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="H2" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
     </row>
     <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="15"/>
-      <c r="H4" s="22" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="16"/>
+      <c r="H4" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="18"/>
-      <c r="H5" s="24" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="19"/>
+      <c r="H5" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
     </row>
     <row r="6" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="19"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="21"/>
-      <c r="H6" s="24" t="s">
+      <c r="A6" s="20"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="22"/>
+      <c r="H6" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="H8" s="10" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="H8" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="H9" s="8" t="s">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="H9" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2751,8 +2751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55C9DC25-BC57-41A3-9745-57893597D3F6}">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="130" zoomScaleSheetLayoutView="160" zoomScalePageLayoutView="10" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="160" zoomScalePageLayoutView="10" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2765,7 +2765,8 @@
     <col min="10" max="11" width="11.33203125" customWidth="1"/>
     <col min="14" max="14" width="14.77734375" customWidth="1"/>
     <col min="15" max="15" width="10.5546875" customWidth="1"/>
-    <col min="17" max="17" width="62.33203125" customWidth="1"/>
+    <col min="16" max="16" width="0" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="62.33203125" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="13.21875" customWidth="1"/>
     <col min="19" max="19" width="16" customWidth="1"/>
   </cols>
@@ -2830,10 +2831,10 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="27">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="7" t="s">
         <v>85</v>
       </c>
       <c r="C2" s="2" t="s">

</xml_diff>